<commit_message>
(update) eStat/qr, eLearning/en, eLearning/kr
</commit_message>
<xml_diff>
--- a/eStat/qr/webAddress.xlsx
+++ b/eStat/qr/webAddress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estat\eStat\QR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estat\eStat\qr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CF3BCB-BDD9-4562-9EEC-97E5EE5645DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6A0C1-F52E-4BCA-BB63-E8A4901EB6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30150" yWindow="390" windowWidth="20085" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41025" yWindow="630" windowWidth="21600" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="333">
   <si>
     <t>estatLecture</t>
   </si>
@@ -270,207 +270,6 @@
     <t>http://www.estat.me/estat/eStatU/index.html</t>
   </si>
   <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/A21Summary_StudentByGender.csv","analysisVar":1,"groupVars":[2,3],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX020301_Raw_Gender.csv","analysisVar":1,"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/A34Raw_Gender.csv","analysisVar":1,"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX020201_Summary_Gender.csv","analysisVar":1,"groupVars":[2],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX020202_OECD_LifeExpectancy.csv","analysisVar":1,"groupVars":[2],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX020203_Summary_StudentByGender.csv","analysisVar":1,"groupVars":[2,3],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX020204_Summary_PopulationByGenderKorea.csv","analysisVar":1,"groupVars":[2,3],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX020205_OECD_ExportImport__2017.csv","analysisVar":1,"groupVars":[2,3],"graphNum":14}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX020302_Raw_MaritalByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR020201_OECD_AlcoholExpenditure_2013.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX030201_Continuous_OtterLength.csv","analysisVar":1,"graphNum":15}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX030202_Continous_TeacherAgeByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":15}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX030203_Continuous_CalorieByHotDog.csv","analysisVar":2,"groupVars":[1],"graphNum":15}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX030301_Continuous_HeightWeightByGender.csv","analysisVar":2,"groupVars":[3],"graphNum":20}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX040101_Categorical_Gender.csv","analysisVar":1,"groupVars":[3],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX040102_Continuous_OtterLength.csv","analysisVar":1,"groupVars":[3],"graphNum":19}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX040201_Categorical_MaritalByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX040202_Continous_TeacherAgeByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":19}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX040310_Continous_TeacherAgeByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":16}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX080103_WageByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":29}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX080104_TypingSpeedEducation.csv","analysisVar":1,"groupVars":[2],"graphNum":29}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX090101_EnglishScoreByGrade.csv","analysisVar":2,"groupVars":[1],"graphNum":33}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX090201_GasMileage.csv","analysisVar":3,"groupVars":[1],"graphNum":33}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX090301_YieldByRiceFertilizer.csv","analysisVar":3,"groupVars":[2,1],"graphNum":33}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX100201_ScoreByDept.csv","analysisVar":2,"groupVars":[1],"graphNum":29}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX110201_GlassesByGender.csv","analysisVar":1,"groupVars":[2,3],"graphNum":14}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX110202_BeverageByRegion.csv","analysisVar":1,"groupVars":[2,3,4],"graphNum":14}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX120101_SalesByAdvertise.csv","analysisVar":2,"groupVars":[1],"graphNum":20}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX120104_Iris.csv","analysisVar":2,"groupVars":[3,4,5],"graphNum":35}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX120301_TreeVolume.csv","analysisVar":3,"groupVars":[1,2],"graphNum":35}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/Ch3_Ex_Mixed_Survey.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR020202_WORLD_ObesityRatio_Age15over__2017.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR020203_Rdatasets_VADeaths.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR020204_OECD_NationalIncome__2017.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030205_Rdatasets_PlantGrowth.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR020205_Summary_TemperatureBySeason.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR020301_Raw_MathPreferenceByGender.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR020302_Raw_MathPreferenceByGender.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030201_Continuous_BikeRoad.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030202_Rdatasets_Rivers.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030203_Rdatasets_Precip.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030204_Continuous_ToothCleanByBrushMethod.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030206_Rdatasets_InsectSprays.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030301_Rdatasets_faithful.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030302_Continuous_IncomeAge.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR040101_Categorical_VegetablePrefByGender.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR030303_Rdatasets_Mtcars.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR040102_Continuous_LibraryVisitorAge.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR040201_Categorical_VegetablePrefByGender.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR040202_Continuous_ToothCleanByBrushMethod.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR040301_Continuous_OtterLength.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR040302_Rdatasets_ToothGrowth.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR070101_Weight.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR080101_ToothCleanByBrushMethod.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR080102_CoupleAge.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR090101_Rdatasets_PlantGrowth.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR090201_WheatAreaYield.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR090301_LifeByTemeratureHumidity.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR100101_CompetencyScore.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR100201_ScoreByMethod.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR100202_DifferenceOfMileage.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR100301_ScoreByMixingMethod.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR110102_OtterLength.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR110201_TV_Reading.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR120101_MidtermFinal.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR120102_SomkingObesityExercise.csv","graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/PR120301_SomkingObesityExercise.csv","graphNum":1}</t>
-  </si>
-  <si>
     <t>http://www.estat.me/estat/eStatU/63SampleEng.htm</t>
   </si>
   <si>
@@ -603,27 +402,9 @@
     <t>http://www.estat.me/estat/eStatU/32RegressionEng.htm</t>
   </si>
   <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX040301_Continuous_QuizScore.csv","analysisVar":1,"graphNum":15}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX070104_Height.csv","analysisVar":1,"graphNum":25}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX100202_AgeOfCouple.csv","analysisVar":1,"graphNum":1}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX100101_CookieWeight.csv","analysisVar":1,"graphNum":25}</t>
-  </si>
-  <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX110102_AgeOfLibraryVisitor.csv","analysisVar":1,"graphNum":19}</t>
-  </si>
-  <si>
     <t>EX080202_WageByGender.csv</t>
   </si>
   <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX080103_WageByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":31}</t>
-  </si>
-  <si>
     <t>eStatH_01BarChart</t>
   </si>
   <si>
@@ -756,9 +537,6 @@
     <t>http://www.estat.me/estat/eStatH/32RegressionEng.htm</t>
   </si>
   <si>
-    <t>http://www.estat.me/estat/eStat/?json={"dataURL":"../Example/eBook/EX100301_JobSatisfaction.csv","analysisVar":2,"groupVars":[1],"graphNum":33}</t>
-  </si>
-  <si>
     <t>eStatH_40Pascal</t>
   </si>
   <si>
@@ -1018,6 +796,234 @@
   </si>
   <si>
     <t>eStatU_10DotGraph</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/A21Summary_StudentByGender.csv","analysisVar":1,"groupVars":[2,3],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/A34Raw_Gender.csv","analysisVar":1,"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/Ch3_Ex_Mixed_Survey.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX020201_Summary_Gender.csv","analysisVar":1,"groupVars":[2],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX020202_OECD_LifeExpectancy.csv","analysisVar":1,"groupVars":[2],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX020203_Summary_StudentByGender.csv","analysisVar":1,"groupVars":[2,3],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX020204_Summary_PopulationByGenderKorea.csv","analysisVar":1,"groupVars":[2,3],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX020205_OECD_ExportImport__2017.csv","analysisVar":1,"groupVars":[2,3],"graphNum":14}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX020301_Raw_Gender.csv","analysisVar":1,"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX020302_Raw_MaritalByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX030201_Continuous_OtterLength.csv","analysisVar":1,"graphNum":15}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX030202_Continous_TeacherAgeByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":15}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX030203_Continuous_CalorieByHotDog.csv","analysisVar":2,"groupVars":[1],"graphNum":15}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX030301_Continuous_HeightWeightByGender.csv","analysisVar":2,"groupVars":[3],"graphNum":20}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX040101_Categorical_Gender.csv","analysisVar":1,"groupVars":[3],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX040102_Continuous_OtterLength.csv","analysisVar":1,"groupVars":[3],"graphNum":19}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX040201_Categorical_MaritalByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX040202_Continous_TeacherAgeByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":19}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX040301_Continuous_QuizScore.csv","analysisVar":1,"graphNum":15}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX040310_Continous_TeacherAgeByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":16}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX070104_Height.csv","analysisVar":1,"graphNum":25}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX080103_WageByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":29}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX080104_TypingSpeedEducation.csv","analysisVar":1,"groupVars":[2],"graphNum":29}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX080103_WageByGender.csv","analysisVar":2,"groupVars":[1],"graphNum":31}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX090101_EnglishScoreByGrade.csv","analysisVar":2,"groupVars":[1],"graphNum":33}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX090201_GasMileage.csv","analysisVar":3,"groupVars":[1],"graphNum":33}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX090301_YieldByRiceFertilizer.csv","analysisVar":3,"groupVars":[2,1],"graphNum":33}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX100101_CookieWeight.csv","analysisVar":1,"graphNum":25}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX100201_ScoreByDept.csv","analysisVar":2,"groupVars":[1],"graphNum":29}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX100202_AgeOfCouple.csv","analysisVar":1,"graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX100301_JobSatisfaction.csv","analysisVar":2,"groupVars":[1],"graphNum":33}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX110102_AgeOfLibraryVisitor.csv","analysisVar":1,"graphNum":19}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX110201_GlassesByGender.csv","analysisVar":1,"groupVars":[2,3],"graphNum":14}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX110202_BeverageByRegion.csv","analysisVar":1,"groupVars":[2,3,4],"graphNum":14}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX120101_SalesByAdvertise.csv","analysisVar":2,"groupVars":[1],"graphNum":20}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX120104_Iris.csv","analysisVar":2,"groupVars":[3,4,5],"graphNum":35}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX120301_TreeVolume.csv","analysisVar":3,"groupVars":[1,2],"graphNum":35}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR020201_OECD_AlcoholExpenditure_2013.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR020202_WORLD_ObesityRatio_Age15over__2017.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR020203_Rdatasets_VADeaths.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR020204_OECD_NationalIncome__2017.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR020205_Summary_TemperatureBySeason.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR020301_Raw_MathPreferenceByGender.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR020302_Raw_MathPreferenceByGender.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030201_Continuous_BikeRoad.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030202_Rdatasets_Rivers.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030203_Rdatasets_Precip.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030204_Continuous_ToothCleanByBrushMethod.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030205_Rdatasets_PlantGrowth.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030206_Rdatasets_InsectSprays.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030301_Rdatasets_faithful.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030302_Continuous_IncomeAge.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR030303_Rdatasets_Mtcars.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR040101_Categorical_VegetablePrefByGender.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR040102_Continuous_LibraryVisitorAge.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR040201_Categorical_VegetablePrefByGender.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR040202_Continuous_ToothCleanByBrushMethod.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR040301_Continuous_OtterLength.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR040302_Rdatasets_ToothGrowth.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR070101_Weight.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR080101_ToothCleanByBrushMethod.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR080102_CoupleAge.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR090101_Rdatasets_PlantGrowth.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR090201_WheatAreaYield.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR090301_LifeByTemeratureHumidity.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR100101_CompetencyScore.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR100201_ScoreByMethod.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR100202_DifferenceOfMileage.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR100301_ScoreByMixingMethod.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR110102_OtterLength.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR110201_TV_Reading.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR120101_MidtermFinal.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR120102_SomkingObesityExercise.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/PR120301_SomkingObesityExercise.csv","graphNum":1}</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStat/indexU.html?json={"dataURL":"../Example/eBook/EX070104_Height.csv","analysisVar":1,"graphNum":27}</t>
+  </si>
+  <si>
+    <t>EX070202_Height.csv</t>
   </si>
 </sst>
 </file>
@@ -1399,10 +1405,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B174"/>
+  <dimension ref="A1:B175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,15 +1454,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>83</v>
+      <c r="B7" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1464,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1472,7 +1478,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1480,7 +1486,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1488,7 +1494,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1496,7 +1502,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -1504,7 +1510,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1512,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -1520,7 +1526,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1528,7 +1534,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1536,7 +1542,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1544,7 +1550,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1552,7 +1558,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1560,7 +1566,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1568,7 +1574,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1576,7 +1582,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1584,7 +1590,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1592,7 +1598,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>192</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1600,7 +1606,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1608,1152 +1614,1160 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>100</v>
+        <v>332</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>198</v>
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>102</v>
+        <v>125</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>195</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>194</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>243</v>
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" t="s">
-        <v>196</v>
+        <v>32</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="B43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" t="s">
-        <v>90</v>
+      <c r="B44" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
+        <v>298</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>299</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>302</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>304</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>306</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>309</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
+        <v>310</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>311</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>313</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>316</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>135</v>
+        <v>317</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>318</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>319</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>321</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>322</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>323</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>324</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>325</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>326</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>327</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B80" t="s">
-        <v>146</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>75</v>
       </c>
-      <c r="B81" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>238</v>
+      <c r="B82" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>325</v>
+      <c r="A84" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>231</v>
+      <c r="A85" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>226</v>
+        <v>152</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>232</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
-        <v>227</v>
+        <v>153</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>233</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
-        <v>228</v>
+        <v>154</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>234</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
-        <v>230</v>
+        <v>155</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>237</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
-        <v>229</v>
+        <v>157</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
-        <v>240</v>
+        <v>156</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>236</v>
+        <v>162</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>160</v>
+        <v>167</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
-        <v>263</v>
+        <v>188</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>190</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
-        <v>264</v>
+        <v>189</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>191</v>
+        <v>123</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>307</v>
+        <v>190</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>260</v>
+        <v>233</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>310</v>
+        <v>187</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>309</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
-        <v>268</v>
+        <v>193</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
-        <v>269</v>
+        <v>194</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>151</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
-        <v>270</v>
+        <v>195</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
-        <v>271</v>
+        <v>196</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
-        <v>272</v>
+        <v>197</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>311</v>
+        <v>198</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>154</v>
+        <v>238</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
-        <v>274</v>
+        <v>199</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
-        <v>275</v>
+        <v>200</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
-        <v>276</v>
+        <v>201</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>158</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
-        <v>277</v>
+        <v>202</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
-        <v>278</v>
+        <v>203</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
-        <v>279</v>
+        <v>204</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>162</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
-        <v>280</v>
+        <v>205</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
-        <v>281</v>
+        <v>206</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
-        <v>282</v>
+        <v>207</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
-        <v>283</v>
+        <v>208</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>167</v>
+        <v>96</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
-        <v>284</v>
+        <v>209</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>165</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
-        <v>285</v>
+        <v>210</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>166</v>
+        <v>98</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
-        <v>286</v>
+        <v>211</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
-        <v>287</v>
+        <v>212</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>169</v>
+        <v>101</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
-        <v>288</v>
+        <v>213</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>172</v>
+        <v>102</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
-        <v>289</v>
+        <v>214</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
-        <v>290</v>
+        <v>215</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
-        <v>291</v>
+        <v>216</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>171</v>
+        <v>103</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
-        <v>292</v>
+        <v>217</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>174</v>
+        <v>104</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
-        <v>293</v>
+        <v>218</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>175</v>
+        <v>107</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
-        <v>294</v>
+        <v>219</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>176</v>
+        <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
-        <v>295</v>
+        <v>220</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>177</v>
+        <v>109</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
-        <v>296</v>
+        <v>221</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>187</v>
+        <v>110</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
-        <v>297</v>
+        <v>222</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>188</v>
+        <v>120</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
-        <v>298</v>
+        <v>223</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
-        <v>299</v>
+        <v>224</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>184</v>
+        <v>112</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
-        <v>301</v>
+        <v>226</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>185</v>
+        <v>113</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
-        <v>302</v>
+        <v>227</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>181</v>
+        <v>118</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
-        <v>303</v>
+        <v>228</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>186</v>
+        <v>114</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
-        <v>304</v>
+        <v>229</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>182</v>
+        <v>119</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
-        <v>305</v>
+        <v>230</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>178</v>
+        <v>122</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
-        <v>323</v>
+        <v>232</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>183</v>
+        <v>111</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
+      <c r="A142" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>201</v>
-      </c>
+      <c r="A143" s="2"/>
+      <c r="B143" s="2"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>217</v>
+        <v>128</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
-        <v>326</v>
+        <v>143</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>327</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
-        <v>199</v>
+        <v>252</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
-        <v>202</v>
+        <v>126</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>215</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
-        <v>203</v>
+        <v>129</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>221</v>
+        <v>142</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
-        <v>204</v>
+        <v>130</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>222</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>223</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="B151" s="5" t="s">
-        <v>329</v>
+      <c r="A151" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>247</v>
+      <c r="A152" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
-        <v>218</v>
+        <v>172</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>219</v>
+        <v>173</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
-        <v>253</v>
+        <v>145</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
-        <v>252</v>
+        <v>179</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>242</v>
+        <v>168</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
-        <v>251</v>
+        <v>178</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>250</v>
+        <v>169</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
-        <v>248</v>
+        <v>177</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>249</v>
+        <v>176</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
-        <v>255</v>
+        <v>174</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>254</v>
+        <v>175</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
-        <v>244</v>
+        <v>181</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>245</v>
+        <v>180</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>220</v>
+        <v>171</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>207</v>
+        <v>133</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
-        <v>314</v>
+        <v>239</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>257</v>
+        <v>240</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
-        <v>315</v>
+        <v>182</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>258</v>
+        <v>183</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>209</v>
+        <v>241</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="2" t="s">
-        <v>317</v>
+        <v>242</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>210</v>
+        <v>136</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
-        <v>318</v>
+        <v>243</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>211</v>
+        <v>137</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
-        <v>319</v>
+        <v>244</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>212</v>
+        <v>138</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
-        <v>320</v>
+        <v>245</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>213</v>
+        <v>139</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
-        <v>321</v>
+        <v>246</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>259</v>
+        <v>247</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="2"/>
-      <c r="B172" s="2"/>
+      <c r="A172" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B174" s="1" t="s">
-        <v>328</v>
+      <c r="A174" s="2"/>
+      <c r="B174" s="2"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B175" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2761,47 +2775,49 @@
     <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B30" r:id="rId4" xr:uid="{F8D7961E-F258-4FA5-869E-615435136B0E}"/>
-    <hyperlink ref="B143" r:id="rId5" xr:uid="{F1887E5F-E1B9-4A84-9B9E-DDC0A791549C}"/>
-    <hyperlink ref="B146" r:id="rId6" xr:uid="{F62620CB-0F76-435D-8F02-4990C6FA6E2F}"/>
-    <hyperlink ref="B147" r:id="rId7" xr:uid="{2D2D479E-2BC8-45DE-AC48-AB3B303F136F}"/>
-    <hyperlink ref="B148" r:id="rId8" xr:uid="{90F3C80F-F3B7-4D66-A216-6EB9BF4687FC}"/>
-    <hyperlink ref="B149" r:id="rId9" xr:uid="{B8BB09CF-5257-4D72-B3DE-AA4ED0D45388}"/>
-    <hyperlink ref="B150" r:id="rId10" xr:uid="{5A3B1D71-7DC4-466D-BD42-9DA4639A6F7C}"/>
-    <hyperlink ref="B151" r:id="rId11" xr:uid="{B4778807-D645-46D7-A508-45CC403C71EB}"/>
-    <hyperlink ref="B160" r:id="rId12" xr:uid="{2C81A0F1-582F-4F81-A78F-31AE9DF53C7E}"/>
-    <hyperlink ref="B144" r:id="rId13" xr:uid="{63A0D520-F036-4E56-A18F-5DF82F89FACB}"/>
-    <hyperlink ref="B153" r:id="rId14" xr:uid="{095D3079-7E54-4AD1-AE13-D731D8402248}"/>
-    <hyperlink ref="B83" r:id="rId15" xr:uid="{919CEF29-99E8-4D25-842B-D0052EF37549}"/>
-    <hyperlink ref="B85" r:id="rId16" xr:uid="{85376BCA-BA45-4C16-AD62-532F69EFD8EA}"/>
-    <hyperlink ref="B86" r:id="rId17" xr:uid="{11E11649-F346-4B1E-AE28-3F6DC4D3D8E8}"/>
-    <hyperlink ref="B87" r:id="rId18" xr:uid="{A5311A07-65A8-4357-BA1A-2A354D6FF251}"/>
-    <hyperlink ref="B88" r:id="rId19" xr:uid="{01B4AAA8-7F20-4025-9D6A-2AE22F93FE86}"/>
-    <hyperlink ref="B91" r:id="rId20" xr:uid="{6E2305E9-1E44-478C-A2B5-6E0045B27138}"/>
-    <hyperlink ref="B90" r:id="rId21" xr:uid="{B3B97DD5-2F8A-4678-AA58-9A9B84B45533}"/>
-    <hyperlink ref="B89" r:id="rId22" xr:uid="{19194B9C-D192-4CD4-A086-2D07B0E4C368}"/>
-    <hyperlink ref="B154" r:id="rId23" xr:uid="{B95774A2-21EA-4F92-89C1-02D4D4F20EBA}"/>
-    <hyperlink ref="B155" r:id="rId24" xr:uid="{0759E9F1-00A7-4074-9EA8-9926EDFF6CA5}"/>
-    <hyperlink ref="B37" r:id="rId25" xr:uid="{0A1BE190-6BB3-4CBD-92E3-6DABE17F4F10}"/>
-    <hyperlink ref="B152" r:id="rId26" xr:uid="{154FE7F7-05A4-417B-B244-687F3D037A70}"/>
-    <hyperlink ref="B157" r:id="rId27" xr:uid="{FE4F0135-1084-4045-8993-28F142534BDE}"/>
-    <hyperlink ref="B159" r:id="rId28" xr:uid="{91568A1D-BD0A-4E49-9033-86A448EB56D1}"/>
-    <hyperlink ref="B156" r:id="rId29" xr:uid="{74AA7DD7-FF24-427F-B407-3FFACC069029}"/>
-    <hyperlink ref="B158" r:id="rId30" xr:uid="{CB4D95CF-7AD4-42FF-9892-FA39432ADE0F}"/>
-    <hyperlink ref="B163" r:id="rId31" xr:uid="{873867A2-CD70-43DE-A876-D99571F3337F}"/>
-    <hyperlink ref="B164" r:id="rId32" xr:uid="{CFA513B5-2A6D-4234-9197-DD021758E3E5}"/>
-    <hyperlink ref="B171" r:id="rId33" xr:uid="{7685040B-E92B-46C3-B52A-6521A98E5CF4}"/>
-    <hyperlink ref="B96" r:id="rId34" xr:uid="{D0D78C19-6FF0-4644-86FF-130F1537A1E1}"/>
-    <hyperlink ref="B98" r:id="rId35" xr:uid="{C4184651-E51F-4A62-919F-746AE264531A}"/>
-    <hyperlink ref="B99" r:id="rId36" xr:uid="{51C5A23F-B156-468F-9B14-1F949A3D4F5D}"/>
-    <hyperlink ref="B95" r:id="rId37" xr:uid="{83537CDB-74E4-49AB-A77A-5EF10F621C21}"/>
-    <hyperlink ref="B106" r:id="rId38" xr:uid="{781A8CE8-81F1-4C9E-9BD3-A410728F3F4A}"/>
-    <hyperlink ref="B97" r:id="rId39" xr:uid="{CF13D62F-CBDC-44EC-AD11-5BBDDB6EE60B}"/>
-    <hyperlink ref="B84" r:id="rId40" xr:uid="{296BB1BC-E26C-4F9A-A677-B88C1BAAF5C3}"/>
-    <hyperlink ref="B145" r:id="rId41" xr:uid="{690C20CB-9B4E-40F4-B5DC-E157F006C9D3}"/>
-    <hyperlink ref="B174" r:id="rId42" xr:uid="{66B8009F-8B11-4B3D-B865-6E4D9CE39FB2}"/>
+    <hyperlink ref="B31" r:id="rId4" display="http://www.estat.me/estat/eStat/?json={&quot;dataURL&quot;:&quot;../Example/eBook/EX080103_WageByGender.csv&quot;,&quot;analysisVar&quot;:2,&quot;groupVars&quot;:[1],&quot;graphNum&quot;:31}" xr:uid="{F8D7961E-F258-4FA5-869E-615435136B0E}"/>
+    <hyperlink ref="B144" r:id="rId5" xr:uid="{F1887E5F-E1B9-4A84-9B9E-DDC0A791549C}"/>
+    <hyperlink ref="B147" r:id="rId6" xr:uid="{F62620CB-0F76-435D-8F02-4990C6FA6E2F}"/>
+    <hyperlink ref="B148" r:id="rId7" xr:uid="{2D2D479E-2BC8-45DE-AC48-AB3B303F136F}"/>
+    <hyperlink ref="B149" r:id="rId8" xr:uid="{90F3C80F-F3B7-4D66-A216-6EB9BF4687FC}"/>
+    <hyperlink ref="B150" r:id="rId9" xr:uid="{B8BB09CF-5257-4D72-B3DE-AA4ED0D45388}"/>
+    <hyperlink ref="B151" r:id="rId10" xr:uid="{5A3B1D71-7DC4-466D-BD42-9DA4639A6F7C}"/>
+    <hyperlink ref="B152" r:id="rId11" xr:uid="{B4778807-D645-46D7-A508-45CC403C71EB}"/>
+    <hyperlink ref="B161" r:id="rId12" xr:uid="{2C81A0F1-582F-4F81-A78F-31AE9DF53C7E}"/>
+    <hyperlink ref="B145" r:id="rId13" xr:uid="{63A0D520-F036-4E56-A18F-5DF82F89FACB}"/>
+    <hyperlink ref="B154" r:id="rId14" xr:uid="{095D3079-7E54-4AD1-AE13-D731D8402248}"/>
+    <hyperlink ref="B84" r:id="rId15" xr:uid="{919CEF29-99E8-4D25-842B-D0052EF37549}"/>
+    <hyperlink ref="B86" r:id="rId16" xr:uid="{85376BCA-BA45-4C16-AD62-532F69EFD8EA}"/>
+    <hyperlink ref="B87" r:id="rId17" xr:uid="{11E11649-F346-4B1E-AE28-3F6DC4D3D8E8}"/>
+    <hyperlink ref="B88" r:id="rId18" xr:uid="{A5311A07-65A8-4357-BA1A-2A354D6FF251}"/>
+    <hyperlink ref="B89" r:id="rId19" xr:uid="{01B4AAA8-7F20-4025-9D6A-2AE22F93FE86}"/>
+    <hyperlink ref="B92" r:id="rId20" xr:uid="{6E2305E9-1E44-478C-A2B5-6E0045B27138}"/>
+    <hyperlink ref="B91" r:id="rId21" xr:uid="{B3B97DD5-2F8A-4678-AA58-9A9B84B45533}"/>
+    <hyperlink ref="B90" r:id="rId22" xr:uid="{19194B9C-D192-4CD4-A086-2D07B0E4C368}"/>
+    <hyperlink ref="B155" r:id="rId23" xr:uid="{B95774A2-21EA-4F92-89C1-02D4D4F20EBA}"/>
+    <hyperlink ref="B156" r:id="rId24" xr:uid="{0759E9F1-00A7-4074-9EA8-9926EDFF6CA5}"/>
+    <hyperlink ref="B38" r:id="rId25" display="http://www.estat.me/estat/eStat/?json={&quot;dataURL&quot;:&quot;../Example/eBook/EX100301_JobSatisfaction.csv&quot;,&quot;analysisVar&quot;:2,&quot;groupVars&quot;:[1],&quot;graphNum&quot;:33}" xr:uid="{0A1BE190-6BB3-4CBD-92E3-6DABE17F4F10}"/>
+    <hyperlink ref="B153" r:id="rId26" xr:uid="{154FE7F7-05A4-417B-B244-687F3D037A70}"/>
+    <hyperlink ref="B158" r:id="rId27" xr:uid="{FE4F0135-1084-4045-8993-28F142534BDE}"/>
+    <hyperlink ref="B160" r:id="rId28" xr:uid="{91568A1D-BD0A-4E49-9033-86A448EB56D1}"/>
+    <hyperlink ref="B157" r:id="rId29" xr:uid="{74AA7DD7-FF24-427F-B407-3FFACC069029}"/>
+    <hyperlink ref="B159" r:id="rId30" xr:uid="{CB4D95CF-7AD4-42FF-9892-FA39432ADE0F}"/>
+    <hyperlink ref="B164" r:id="rId31" xr:uid="{873867A2-CD70-43DE-A876-D99571F3337F}"/>
+    <hyperlink ref="B165" r:id="rId32" xr:uid="{CFA513B5-2A6D-4234-9197-DD021758E3E5}"/>
+    <hyperlink ref="B172" r:id="rId33" xr:uid="{7685040B-E92B-46C3-B52A-6521A98E5CF4}"/>
+    <hyperlink ref="B97" r:id="rId34" xr:uid="{D0D78C19-6FF0-4644-86FF-130F1537A1E1}"/>
+    <hyperlink ref="B99" r:id="rId35" xr:uid="{C4184651-E51F-4A62-919F-746AE264531A}"/>
+    <hyperlink ref="B100" r:id="rId36" xr:uid="{51C5A23F-B156-468F-9B14-1F949A3D4F5D}"/>
+    <hyperlink ref="B96" r:id="rId37" xr:uid="{83537CDB-74E4-49AB-A77A-5EF10F621C21}"/>
+    <hyperlink ref="B107" r:id="rId38" xr:uid="{781A8CE8-81F1-4C9E-9BD3-A410728F3F4A}"/>
+    <hyperlink ref="B98" r:id="rId39" xr:uid="{CF13D62F-CBDC-44EC-AD11-5BBDDB6EE60B}"/>
+    <hyperlink ref="B85" r:id="rId40" xr:uid="{296BB1BC-E26C-4F9A-A677-B88C1BAAF5C3}"/>
+    <hyperlink ref="B146" r:id="rId41" xr:uid="{690C20CB-9B4E-40F4-B5DC-E157F006C9D3}"/>
+    <hyperlink ref="B175" r:id="rId42" xr:uid="{66B8009F-8B11-4B3D-B865-6E4D9CE39FB2}"/>
+    <hyperlink ref="B7" r:id="rId43" display="http://www.estat.me/estat/eStat/?json={&quot;dataURL&quot;:&quot;../Example/eBook/A34Raw_Gender.csv&quot;,&quot;analysisVar&quot;:1,&quot;graphNum&quot;:1}" xr:uid="{81460A8A-E215-40F5-A4E8-DDB5B8ABEFFF}"/>
+    <hyperlink ref="B28" r:id="rId44" xr:uid="{57B2F9CE-C781-45E3-885A-CDE97331B3D6}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId43"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>